<commit_message>
Move Import/Export Type to Power_ImpExpHubs.xlsx
</commit_message>
<xml_diff>
--- a/data/example/Power_ImpExpHubs.xlsx
+++ b/data/example/Power_ImpExpHubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C42EC34-C798-4E7D-AAC4-5F0491DB8319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051EB8F1-59FC-4286-BB7D-D2FF783A00A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="857" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power ImpExp" sheetId="117" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>i</t>
   </si>
@@ -145,6 +145,36 @@
   </si>
   <si>
     <t>Maximum power export</t>
+  </si>
+  <si>
+    <t>Import Type</t>
+  </si>
+  <si>
+    <t>Export Type</t>
+  </si>
+  <si>
+    <t>[ImpFix or ImpMax]</t>
+  </si>
+  <si>
+    <t>[ExpFix or ExpMax]</t>
+  </si>
+  <si>
+    <t>ImpFix</t>
+  </si>
+  <si>
+    <t>ExpMax</t>
+  </si>
+  <si>
+    <t>ImpMax</t>
+  </si>
+  <si>
+    <t>ExpFix</t>
+  </si>
+  <si>
+    <t>Determines wether ImpExp will be enforced as == ('Fix') or &gt;= ('Max')</t>
+  </si>
+  <si>
+    <t>Only ImpFix or ImpMax per hub, and ExpFix or ExpMax per hub</t>
   </si>
 </sst>
 </file>
@@ -715,7 +745,7 @@
   <sheetPr codeName="Tabelle11">
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
@@ -726,15 +756,16 @@
     <col min="3" max="3" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="7"/>
+    <col min="6" max="7" width="31.28515625" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>10</v>
       </c>
@@ -747,8 +778,14 @@
       <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="F3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
@@ -761,16 +798,24 @@
       <c r="E4" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
+      <c r="F5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="9" t="s">
@@ -779,8 +824,14 @@
       <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
@@ -788,13 +839,19 @@
         <v>1</v>
       </c>
       <c r="D7" s="12">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="E7" s="12">
-        <v>120</v>
+        <v>100</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
@@ -802,13 +859,19 @@
         <v>7</v>
       </c>
       <c r="D8" s="12">
-        <v>175</v>
+        <v>75</v>
       </c>
       <c r="E8" s="12">
         <v>150</v>
       </c>
+      <c r="F8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="9" spans="2:5" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" s="2" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
@@ -816,14 +879,28 @@
         <v>1</v>
       </c>
       <c r="D9" s="12">
+        <v>130</v>
+      </c>
+      <c r="E9" s="12">
         <v>200</v>
       </c>
-      <c r="E9" s="12">
-        <v>125</v>
+      <c r="F9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F9" xr:uid="{D365EAED-D789-4592-BC22-3422DB41908E}">
+      <formula1>"ImpFix, ImpMax"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G9" xr:uid="{3D87F385-E080-416E-899B-29A146885A8C}">
+      <formula1>"ExpFix, ExpMax"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -831,6 +908,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -976,35 +1068,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1026,9 +1093,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>